<commit_message>
Penambahan Grade, Predikat, Tahun Wisuda
</commit_message>
<xml_diff>
--- a/Data_Wisudawan_Cleansheet.xlsx
+++ b/Data_Wisudawan_Cleansheet.xlsx
@@ -436,32 +436,32 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nim</t>
+          <t>nim</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nama Mahasiswa</t>
+          <t>nama mahasiswa</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Program Studi</t>
+          <t>program studi</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Ipk</t>
+          <t>ipk</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Lama Studi (Semester)</t>
+          <t>lama studi (semester)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Tahun Wisuda</t>
+          <t>tahun wisuda</t>
         </is>
       </c>
     </row>

</xml_diff>